<commit_message>
Mise a jour du suivit
</commit_message>
<xml_diff>
--- a/Sprint2/B65_S2_Suivi_HuotVincent.xlsx
+++ b/Sprint2/B65_S2_Suivi_HuotVincent.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Brain stopped working\Synthèse\Synth-se\Sprint2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Brain stopped working\Synthèse\Synthese\Sprint2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9DAEB1-B24F-49A4-9D1B-4D13B553F841}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE80CFA8-8CD7-44AC-BFCF-FD957B256ED1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{095FB179-6C06-4AD7-A176-EB372BB9DE22}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="50">
   <si>
     <t>Tâche</t>
   </si>
@@ -183,6 +183,9 @@
   </si>
   <si>
     <t>Raison du retard (si nécessaire)</t>
+  </si>
+  <si>
+    <t>Moins simple que prévus : pas de fonction dédié + problème a définir l'emplacement du sample du fichier pendant la lecture</t>
   </si>
 </sst>
 </file>
@@ -507,9 +510,8 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="64">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+  <dxfs count="45">
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -517,6 +519,16 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -531,7 +543,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -539,22 +550,9 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -594,228 +592,20 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -965,6 +755,68 @@
         </vertical>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1403,7 +1255,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B9E80AAD-BAB7-452C-B918-C4BC08F29F45}" name="Table1" displayName="Table1" ref="B2:F37" headerRowDxfId="54" dataDxfId="52" headerRowBorderDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B9E80AAD-BAB7-452C-B918-C4BC08F29F45}" name="Table1" displayName="Table1" ref="B2:F37" headerRowDxfId="35" dataDxfId="33" headerRowBorderDxfId="34">
   <autoFilter ref="B2:F37" xr:uid="{86EE57DA-BF06-4C66-BB51-2A0288918067}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1412,18 +1264,18 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{0A91E22B-1B94-4D8E-B13D-E7630042D129}" name="ID" totalsRowLabel="Total" dataDxfId="51" totalsRowDxfId="50"/>
-    <tableColumn id="2" xr3:uid="{972D5420-A2A0-4367-95FE-C468603F1BB2}" name="Tâche" dataDxfId="49" totalsRowDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{74469926-D14D-4EA0-B99C-C62397E3AEF0}" name="Importance" dataDxfId="47" totalsRowDxfId="46"/>
-    <tableColumn id="4" xr3:uid="{A6796943-1F6D-43DC-91DD-6F733CACA5AD}" name="Prérequis" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="5" xr3:uid="{83222E1A-71E0-4765-BA1F-64A63F3971AF}" name="Temps requis" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="1" xr3:uid="{0A91E22B-1B94-4D8E-B13D-E7630042D129}" name="ID" totalsRowLabel="Total" dataDxfId="32" totalsRowDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{972D5420-A2A0-4367-95FE-C468603F1BB2}" name="Tâche" dataDxfId="30" totalsRowDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{74469926-D14D-4EA0-B99C-C62397E3AEF0}" name="Importance" dataDxfId="28" totalsRowDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{A6796943-1F6D-43DC-91DD-6F733CACA5AD}" name="Prérequis" dataDxfId="26" totalsRowDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{83222E1A-71E0-4765-BA1F-64A63F3971AF}" name="Temps requis" dataDxfId="24" totalsRowDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{43CE93C2-2824-4706-BC62-20A5DDDF15C0}" name="Table13" displayName="Table13" ref="B2:G37" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{43CE93C2-2824-4706-BC62-20A5DDDF15C0}" name="Table13" displayName="Table13" ref="B2:G37" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13">
   <autoFilter ref="B2:G37" xr:uid="{8CA08DB7-B7D2-4330-90AE-CB3D9316DC3B}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1433,12 +1285,12 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{291097C9-E400-47B0-B2A3-69203B0D7A2D}" name="ID" totalsRowLabel="Total" dataDxfId="38" totalsRowDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{DE3E80C2-9C01-4501-9F6A-30E7445332C5}" name="Tâche" dataDxfId="36" totalsRowDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{5BB79306-DB2C-4B8F-A79D-412BF8339CDC}" name="État" dataDxfId="34" totalsRowDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{427233C1-2691-4DEF-8395-9F2158A5E560}" name="Avancement" dataDxfId="2" totalsRowDxfId="5" dataCellStyle="Percent"/>
-    <tableColumn id="5" xr3:uid="{3135688F-0FF7-4089-887D-6061C2647E5D}" name="temp investi" dataDxfId="1" totalsRowDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{97A1ED9D-A557-4ADA-B362-399FA7E37D6D}" name="Raison du retard (si nécessaire)" dataDxfId="0" totalsRowDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{291097C9-E400-47B0-B2A3-69203B0D7A2D}" name="ID" totalsRowLabel="Total" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{DE3E80C2-9C01-4501-9F6A-30E7445332C5}" name="Tâche" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{5BB79306-DB2C-4B8F-A79D-412BF8339CDC}" name="État" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{427233C1-2691-4DEF-8395-9F2158A5E560}" name="Avancement" dataDxfId="5" totalsRowDxfId="4" dataCellStyle="Percent"/>
+    <tableColumn id="5" xr3:uid="{3135688F-0FF7-4089-887D-6061C2647E5D}" name="temp investi" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{97A1ED9D-A557-4ADA-B362-399FA7E37D6D}" name="Raison du retard (si nécessaire)" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2545,7 +2397,7 @@
   <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -2597,12 +2449,14 @@
         <v>4</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E3" s="26">
-        <v>0.3</v>
-      </c>
-      <c r="F3" s="27"/>
+        <v>1</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>10</v>
+      </c>
       <c r="G3" s="28"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2613,11 +2467,13 @@
         <v>5</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E4" s="26"/>
       <c r="F4" s="27"/>
-      <c r="G4" s="28"/>
+      <c r="G4" s="28" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="9">

</xml_diff>

<commit_message>
fixed pitch problem and added per voice playhead visual
</commit_message>
<xml_diff>
--- a/Sprint2/B65_S2_Suivi_HuotVincent.xlsx
+++ b/Sprint2/B65_S2_Suivi_HuotVincent.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Brain stopped working\Synthèse\Synthese\Sprint2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CBCDD87-B290-4690-9A53-116531450663}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F1371E-B310-484E-ABD3-A632EFB52AA8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="1950" windowWidth="25050" windowHeight="11835" activeTab="1" xr2:uid="{095FB179-6C06-4AD7-A176-EB372BB9DE22}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{095FB179-6C06-4AD7-A176-EB372BB9DE22}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1 - Planification" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="53">
   <si>
     <t>Tâche</t>
   </si>
@@ -525,146 +525,6 @@
   <dxfs count="45">
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="1"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="1"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="0"/>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="3" tint="-0.249977111117893"/>
@@ -910,6 +770,68 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="3" tint="-0.249977111117893"/>
@@ -1132,6 +1054,84 @@
         </vertical>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="1"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="1"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="0"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1267,7 +1267,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B9E80AAD-BAB7-452C-B918-C4BC08F29F45}" name="Table1" displayName="Table1" ref="B2:F37" headerRowDxfId="44" dataDxfId="42" headerRowBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B9E80AAD-BAB7-452C-B918-C4BC08F29F45}" name="Table1" displayName="Table1" ref="B2:F37" headerRowDxfId="35" dataDxfId="33" headerRowBorderDxfId="34">
   <autoFilter ref="B2:F37" xr:uid="{86EE57DA-BF06-4C66-BB51-2A0288918067}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1276,18 +1276,18 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{0A91E22B-1B94-4D8E-B13D-E7630042D129}" name="ID" totalsRowLabel="Total" dataDxfId="41" totalsRowDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{972D5420-A2A0-4367-95FE-C468603F1BB2}" name="Tâche" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{74469926-D14D-4EA0-B99C-C62397E3AEF0}" name="Importance" dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{A6796943-1F6D-43DC-91DD-6F733CACA5AD}" name="Prérequis" dataDxfId="35" totalsRowDxfId="34"/>
-    <tableColumn id="5" xr3:uid="{83222E1A-71E0-4765-BA1F-64A63F3971AF}" name="Temps requis" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{0A91E22B-1B94-4D8E-B13D-E7630042D129}" name="ID" totalsRowLabel="Total" dataDxfId="32" totalsRowDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{972D5420-A2A0-4367-95FE-C468603F1BB2}" name="Tâche" dataDxfId="30" totalsRowDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{74469926-D14D-4EA0-B99C-C62397E3AEF0}" name="Importance" dataDxfId="28" totalsRowDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{A6796943-1F6D-43DC-91DD-6F733CACA5AD}" name="Prérequis" dataDxfId="26" totalsRowDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{83222E1A-71E0-4765-BA1F-64A63F3971AF}" name="Temps requis" dataDxfId="24" totalsRowDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{43CE93C2-2824-4706-BC62-20A5DDDF15C0}" name="Table13" displayName="Table13" ref="B2:G38" headerRowDxfId="31" dataDxfId="29" headerRowBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{43CE93C2-2824-4706-BC62-20A5DDDF15C0}" name="Table13" displayName="Table13" ref="B2:G38" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13">
   <autoFilter ref="B2:G38" xr:uid="{8CA08DB7-B7D2-4330-90AE-CB3D9316DC3B}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1297,12 +1297,12 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{291097C9-E400-47B0-B2A3-69203B0D7A2D}" name="ID" totalsRowLabel="Total" dataDxfId="28" totalsRowDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{DE3E80C2-9C01-4501-9F6A-30E7445332C5}" name="Tâche" dataDxfId="26" totalsRowDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{5BB79306-DB2C-4B8F-A79D-412BF8339CDC}" name="État" dataDxfId="24" totalsRowDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{427233C1-2691-4DEF-8395-9F2158A5E560}" name="Avancement" dataDxfId="22" totalsRowDxfId="21" dataCellStyle="Percent"/>
-    <tableColumn id="5" xr3:uid="{3135688F-0FF7-4089-887D-6061C2647E5D}" name="temp investi" dataDxfId="20" totalsRowDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{97A1ED9D-A557-4ADA-B362-399FA7E37D6D}" name="Raison du retard (si nécessaire)" dataDxfId="18" totalsRowDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{291097C9-E400-47B0-B2A3-69203B0D7A2D}" name="ID" totalsRowLabel="Total" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{DE3E80C2-9C01-4501-9F6A-30E7445332C5}" name="Tâche" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{5BB79306-DB2C-4B8F-A79D-412BF8339CDC}" name="État" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{427233C1-2691-4DEF-8395-9F2158A5E560}" name="Avancement" dataDxfId="5" totalsRowDxfId="4" dataCellStyle="Percent"/>
+    <tableColumn id="5" xr3:uid="{3135688F-0FF7-4089-887D-6061C2647E5D}" name="temp investi" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{97A1ED9D-A557-4ADA-B362-399FA7E37D6D}" name="Raison du retard (si nécessaire)" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2408,8 +2408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18ADBC28-B31F-43DC-9A5D-D49110B3517C}">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -2517,12 +2517,14 @@
         <v>50</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" s="26">
-        <v>0</v>
-      </c>
-      <c r="F6" s="27"/>
+        <v>1</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>12</v>
+      </c>
       <c r="G6" s="28" t="s">
         <v>52</v>
       </c>
@@ -2535,10 +2537,14 @@
         <v>7</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" s="26"/>
-      <c r="F7" s="27"/>
+        <v>43</v>
+      </c>
+      <c r="E7" s="26">
+        <v>1</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>11</v>
+      </c>
       <c r="G7" s="28"/>
     </row>
     <row r="8" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2549,7 +2555,7 @@
         <v>16</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E8" s="26"/>
       <c r="F8" s="27"/>

</xml_diff>

<commit_message>
Updated sprint 2 document
</commit_message>
<xml_diff>
--- a/Sprint2/B65_S2_Suivi_HuotVincent.xlsx
+++ b/Sprint2/B65_S2_Suivi_HuotVincent.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Brain stopped working\Synthèse\Synthese\Sprint2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F1371E-B310-484E-ABD3-A632EFB52AA8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F608C2D-5078-4428-9406-DCC22F4B7126}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{095FB179-6C06-4AD7-A176-EB372BB9DE22}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="53">
   <si>
     <t>Tâche</t>
   </si>
@@ -2409,7 +2409,7 @@
   <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -2555,10 +2555,14 @@
         <v>16</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="26"/>
-      <c r="F8" s="27"/>
+        <v>43</v>
+      </c>
+      <c r="E8" s="26">
+        <v>1</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>10</v>
+      </c>
       <c r="G8" s="28"/>
     </row>
     <row r="9" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Management of Pan, volume, and length of individual grains
</commit_message>
<xml_diff>
--- a/Sprint2/B65_S2_Suivi_HuotVincent.xlsx
+++ b/Sprint2/B65_S2_Suivi_HuotVincent.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Brain stopped working\Synthèse\Synthese\Sprint2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F608C2D-5078-4428-9406-DCC22F4B7126}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FA28ED-7CB6-4C38-AA83-352801ABBAEC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{095FB179-6C06-4AD7-A176-EB372BB9DE22}"/>
+    <workbookView xWindow="810" yWindow="-16320" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{095FB179-6C06-4AD7-A176-EB372BB9DE22}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1 - Planification" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="55">
   <si>
     <t>Tâche</t>
   </si>
@@ -195,6 +195,12 @@
   </si>
   <si>
     <t>Due a un changement de plan, il faut que je gère les informations MIDI autrement. Cette nouvelle étape est donc nécessaire.</t>
+  </si>
+  <si>
+    <t>Vitesse de lecture = pitch dans ce context.</t>
+  </si>
+  <si>
+    <t>ADSR a été fait plus tôt que prévu puisque façile a implémenter avec le MIDI</t>
   </si>
 </sst>
 </file>
@@ -2409,7 +2415,7 @@
   <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -2573,10 +2579,14 @@
         <v>17</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" s="26"/>
-      <c r="F9" s="27"/>
+        <v>43</v>
+      </c>
+      <c r="E9" s="26">
+        <v>1</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>10</v>
+      </c>
       <c r="G9" s="28"/>
     </row>
     <row r="10" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2587,10 +2597,14 @@
         <v>18</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10" s="26"/>
-      <c r="F10" s="27"/>
+        <v>43</v>
+      </c>
+      <c r="E10" s="26">
+        <v>1</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>10</v>
+      </c>
       <c r="G10" s="28"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2601,10 +2615,14 @@
         <v>19</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="26"/>
-      <c r="F11" s="27"/>
+        <v>43</v>
+      </c>
+      <c r="E11" s="26">
+        <v>1</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>10</v>
+      </c>
       <c r="G11" s="28"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2615,11 +2633,17 @@
         <v>15</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" s="26"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="28"/>
+        <v>43</v>
+      </c>
+      <c r="E12" s="26">
+        <v>1</v>
+      </c>
+      <c r="F12" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="9">
@@ -2699,10 +2723,14 @@
         <v>31</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E18" s="26"/>
-      <c r="F18" s="27"/>
+        <v>43</v>
+      </c>
+      <c r="E18" s="26">
+        <v>1</v>
+      </c>
+      <c r="F18" s="27" t="s">
+        <v>10</v>
+      </c>
       <c r="G18" s="28"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
@@ -2713,10 +2741,14 @@
         <v>32</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E19" s="26"/>
-      <c r="F19" s="27"/>
+        <v>43</v>
+      </c>
+      <c r="E19" s="26">
+        <v>1</v>
+      </c>
+      <c r="F19" s="27" t="s">
+        <v>10</v>
+      </c>
       <c r="G19" s="28"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
@@ -2727,11 +2759,17 @@
         <v>6</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" s="26"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="28"/>
+        <v>43</v>
+      </c>
+      <c r="E20" s="26">
+        <v>1</v>
+      </c>
+      <c r="F20" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="K20" s="24"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changed structure (added CWGVoice class)
</commit_message>
<xml_diff>
--- a/Sprint2/B65_S2_Suivi_HuotVincent.xlsx
+++ b/Sprint2/B65_S2_Suivi_HuotVincent.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Brain stopped working\Synthèse\Synthese\Sprint2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FA28ED-7CB6-4C38-AA83-352801ABBAEC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E18BD0-F5A2-4E81-8750-9E6ED4D3C905}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-16320" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{095FB179-6C06-4AD7-A176-EB372BB9DE22}"/>
   </bookViews>
@@ -2415,7 +2415,7 @@
   <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -2653,7 +2653,7 @@
         <v>20</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E13" s="26"/>
       <c r="F13" s="27"/>

</xml_diff>

<commit_message>
Added Waveform Panel class and half updated UI
</commit_message>
<xml_diff>
--- a/Sprint2/B65_S2_Suivi_HuotVincent.xlsx
+++ b/Sprint2/B65_S2_Suivi_HuotVincent.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Brain stopped working\Synthèse\Synthese\Sprint2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E18BD0-F5A2-4E81-8750-9E6ED4D3C905}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62DC9475-7986-4BE4-9F47-6169CE978852}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-16320" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{095FB179-6C06-4AD7-A176-EB372BB9DE22}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="56">
   <si>
     <t>Tâche</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>ADSR a été fait plus tôt que prévu puisque façile a implémenter avec le MIDI</t>
+  </si>
+  <si>
+    <t>Retiré. Cause : "Ça sonne pas fameux"</t>
   </si>
 </sst>
 </file>
@@ -2415,7 +2418,7 @@
   <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -2713,7 +2716,9 @@
       </c>
       <c r="E17" s="26"/>
       <c r="F17" s="27"/>
-      <c r="G17" s="28"/>
+      <c r="G17" s="28" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="9">

</xml_diff>

<commit_message>
Finalized project and added VST3 and Standalone releases
</commit_message>
<xml_diff>
--- a/Sprint2/B65_S2_Suivi_HuotVincent.xlsx
+++ b/Sprint2/B65_S2_Suivi_HuotVincent.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Brain stopped working\Synthèse\Synthese\Sprint2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62DC9475-7986-4BE4-9F47-6169CE978852}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3601E9A4-5881-4E01-A92B-2463666DFEF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-16320" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{095FB179-6C06-4AD7-A176-EB372BB9DE22}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="58">
   <si>
     <t>Tâche</t>
   </si>
@@ -204,6 +204,12 @@
   </si>
   <si>
     <t>Retiré. Cause : "Ça sonne pas fameux"</t>
+  </si>
+  <si>
+    <t>Complications lors de création de paramètre VST après construction</t>
+  </si>
+  <si>
+    <t>std::rand() retourne une valeur maximum trop petite</t>
   </si>
 </sst>
 </file>
@@ -2418,7 +2424,7 @@
   <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -2552,7 +2558,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G7" s="28"/>
     </row>
@@ -2656,10 +2662,14 @@
         <v>20</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="26"/>
-      <c r="F13" s="27"/>
+        <v>43</v>
+      </c>
+      <c r="E13" s="26">
+        <v>1</v>
+      </c>
+      <c r="F13" s="27" t="s">
+        <v>11</v>
+      </c>
       <c r="G13" s="28"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2670,11 +2680,17 @@
         <v>21</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14" s="26"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="28"/>
+        <v>43</v>
+      </c>
+      <c r="E14" s="26">
+        <v>1</v>
+      </c>
+      <c r="F14" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="28" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="9">
@@ -2684,10 +2700,14 @@
         <v>23</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" s="26"/>
-      <c r="F15" s="27"/>
+        <v>43</v>
+      </c>
+      <c r="E15" s="26">
+        <v>1</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>10</v>
+      </c>
       <c r="G15" s="28"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2698,10 +2718,14 @@
         <v>22</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="26"/>
-      <c r="F16" s="27"/>
+        <v>43</v>
+      </c>
+      <c r="E16" s="26">
+        <v>1</v>
+      </c>
+      <c r="F16" s="27" t="s">
+        <v>10</v>
+      </c>
       <c r="G16" s="28"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
@@ -2714,8 +2738,12 @@
       <c r="D17" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="26"/>
-      <c r="F17" s="27"/>
+      <c r="E17" s="26">
+        <v>0</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>28</v>
+      </c>
       <c r="G17" s="28" t="s">
         <v>55</v>
       </c>
@@ -2770,7 +2798,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="27" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G20" s="28" t="s">
         <v>54</v>
@@ -2785,10 +2813,14 @@
         <v>33</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21" s="26"/>
-      <c r="F21" s="27"/>
+        <v>43</v>
+      </c>
+      <c r="E21" s="26">
+        <v>1</v>
+      </c>
+      <c r="F21" s="27" t="s">
+        <v>11</v>
+      </c>
       <c r="G21" s="28"/>
       <c r="K21" s="24"/>
     </row>
@@ -2800,11 +2832,17 @@
         <v>34</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E22" s="26"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="28"/>
+        <v>43</v>
+      </c>
+      <c r="E22" s="26">
+        <v>1</v>
+      </c>
+      <c r="F22" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="28" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="9">
@@ -2814,10 +2852,14 @@
         <v>37</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E23" s="26"/>
-      <c r="F23" s="27"/>
+        <v>43</v>
+      </c>
+      <c r="E23" s="26">
+        <v>1</v>
+      </c>
+      <c r="F23" s="27" t="s">
+        <v>10</v>
+      </c>
       <c r="G23" s="28"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
@@ -2828,10 +2870,14 @@
         <v>35</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E24" s="26"/>
-      <c r="F24" s="27"/>
+        <v>43</v>
+      </c>
+      <c r="E24" s="26">
+        <v>1</v>
+      </c>
+      <c r="F24" s="27" t="s">
+        <v>10</v>
+      </c>
       <c r="G24" s="28"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
@@ -2842,10 +2888,14 @@
         <v>36</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E25" s="26"/>
-      <c r="F25" s="27"/>
+        <v>43</v>
+      </c>
+      <c r="E25" s="26">
+        <v>1</v>
+      </c>
+      <c r="F25" s="27" t="s">
+        <v>10</v>
+      </c>
       <c r="G25" s="28"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
@@ -2856,10 +2906,14 @@
         <v>38</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E26" s="26"/>
-      <c r="F26" s="27"/>
+        <v>43</v>
+      </c>
+      <c r="E26" s="26">
+        <v>1</v>
+      </c>
+      <c r="F26" s="27" t="s">
+        <v>10</v>
+      </c>
       <c r="G26" s="28"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
@@ -2870,10 +2924,14 @@
         <v>39</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E27" s="26"/>
-      <c r="F27" s="27"/>
+        <v>43</v>
+      </c>
+      <c r="E27" s="26">
+        <v>1</v>
+      </c>
+      <c r="F27" s="27" t="s">
+        <v>10</v>
+      </c>
       <c r="G27" s="28"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
@@ -2884,10 +2942,14 @@
         <v>40</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E28" s="26"/>
-      <c r="F28" s="27"/>
+        <v>43</v>
+      </c>
+      <c r="E28" s="26">
+        <v>1</v>
+      </c>
+      <c r="F28" s="27" t="s">
+        <v>10</v>
+      </c>
       <c r="G28" s="28"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
@@ -2898,10 +2960,14 @@
         <v>41</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E29" s="26"/>
-      <c r="F29" s="27"/>
+        <v>43</v>
+      </c>
+      <c r="E29" s="26">
+        <v>1</v>
+      </c>
+      <c r="F29" s="27" t="s">
+        <v>10</v>
+      </c>
       <c r="G29" s="28"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">

</xml_diff>